<commit_message>
Feat : BaseAttributeSet 구현
</commit_message>
<xml_diff>
--- a/DesignData/Excel_Masters/EnemyStats_Master.xlsx
+++ b/DesignData/Excel_Masters/EnemyStats_Master.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\UnrealCpp\Paradise\DesignData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\UnrealCpp\Paradise\DesignData\Excel_Masters\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>---</t>
   </si>
@@ -32,9 +32,6 @@
   </si>
   <si>
     <t>RankTypeTag</t>
-  </si>
-  <si>
-    <t>AttackInterval</t>
   </si>
   <si>
     <t>AttackRange</t>
@@ -101,6 +98,13 @@
   <si>
     <t>Zombie</t>
     <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>AttackSpeed</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Cooldown</t>
   </si>
 </sst>
 </file>
@@ -1018,10 +1022,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L2"/>
+  <dimension ref="A1:M2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2:K1048576"/>
+      <selection activeCell="E1" sqref="E1:G1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1029,9 +1033,10 @@
     <col min="2" max="2" width="15.625" customWidth="1"/>
     <col min="3" max="3" width="14.125" customWidth="1"/>
     <col min="4" max="4" width="13.5" customWidth="1"/>
+    <col min="6" max="6" width="9.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1045,51 +1050,54 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="M1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B2" t="s">
-        <v>12</v>
-      </c>
       <c r="C2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E2">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="F2">
         <v>100</v>
       </c>
       <c r="G2">
-        <v>10</v>
+        <v>0.2</v>
       </c>
       <c r="H2">
         <v>10</v>
@@ -1101,36 +1109,42 @@
         <v>10</v>
       </c>
       <c r="K2">
+        <v>10</v>
+      </c>
+      <c r="L2">
         <v>1000</v>
       </c>
-      <c r="L2">
+      <c r="M2">
         <v>0.1</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
-  <dataValidations count="7">
+  <dataValidations count="8">
     <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="중복된 ID (RowName Error)" error="이미 존재하는 ID입니다!_x000a__x000a_RowName(행 이름)은 고유해야 합니다._x000a_(같은 이름을 두 번 쓸 수 없습니다.)" sqref="A1:A1048576">
       <formula1>COUNTIF($A:$A, A1) &lt;= 1</formula1>
     </dataValidation>
-    <dataValidation type="decimal" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="입력 오류 (Time)" error="공격 주기는 0보다 작을 수 없습니다._x000a_단위는 '초(Seconds)' 입니다._x000a_(예: 1.5 = 1.5초마다 공격)" sqref="E1:E1048576">
-      <formula1>0.1</formula1>
+    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="입력 오류" error="음수(-)와 0은 입력할 수 없습니다. 0 보다 큰 숫자를 입력해주세요." sqref="E2:E1048576">
+      <formula1>0</formula1>
     </dataValidation>
     <dataValidation type="decimal" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="입력 오류(Range)" error="공격 사거리는 0보다 작을 수 없습니다._x000a_(예: 100 = 1미터)" sqref="F1:F1048576">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="decimal" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="입력 오류 (Speed)" error="속도는 0보다 작을 수 없습니다._x000a_언리얼 단위(cm/s)입니다._x000a_(예: 100 = 1미터, 600 = 달리기 속도)" sqref="K1:K1048576">
+    <dataValidation type="decimal" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="입력 오류 (Speed)" error="속도는 0보다 작을 수 없습니다._x000a_언리얼 단위(cm/s)입니다._x000a_(예: 100 = 1미터, 600 = 달리기 속도)" sqref="L1:L1048576">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="decimal" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="최소 체력 오류" error="최대 체력(MaxHP)은 최소 1 이상이어야 합니다._x000a_0을 입력하면 유닛이 생성되자마자 죽습니다!" sqref="G1:G1048576">
+    <dataValidation type="decimal" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="최소 체력 오류" error="최대 체력(MaxHP)은 최소 1 이상이어야 합니다._x000a_0을 입력하면 유닛이 생성되자마자 죽습니다!" sqref="H1:H1048576">
       <formula1>1</formula1>
     </dataValidation>
-    <dataValidation type="decimal" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="스탯 입력 오류" error="기본 스탯은 음수(-)일 수 없습니다._x000a_0 이상의 값을 입력해주세요." sqref="H1:H1048576 J1:J1048576 I1:I1048576">
+    <dataValidation type="decimal" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="스탯 입력 오류" error="기본 스탯은 음수(-)일 수 없습니다._x000a_0 이상의 값을 입력해주세요." sqref="I1:K1048576">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="확률 범위 오류 (0~1)" error="확률은 0.0 ~ 1.0 사이의 값만 가능합니다._x000a__x000a_[올바른 예시]_x000a_- 10% -&gt; 0.1 입력_x000a_- 50% -&gt; 0.5 입력_x000a_- 100% -&gt; 1.0 입력" sqref="L1:L1048576">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="확률 범위 오류 (0~1)" error="확률은 0.0 ~ 1.0 사이의 값만 가능합니다._x000a__x000a_[올바른 예시]_x000a_- 10% -&gt; 0.1 입력_x000a_- 50% -&gt; 0.5 입력_x000a_- 100% -&gt; 1.0 입력" sqref="M1:M1048576">
       <formula1>0</formula1>
       <formula2>1</formula2>
+    </dataValidation>
+    <dataValidation type="decimal" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="단위 확인 (Cooldown)" error="쿨타임은 0보다 작을 수 없습니다._x000a__x000a_※ 단위: 초 (Seconds)_x000a_- 1분 = '60' 입력_x000a_- 0.5초 = '0.5' 입력_x000a_- 쿨타임 없음 = '0' 입력_x000a__x000a_밀리초(ms) 단위가 아닙니다! 다시 확인해주세요." sqref="G2:G1048576">
+      <formula1>0</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1178,32 +1192,32 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>